<commit_message>
added comments, adjusted variable names
</commit_message>
<xml_diff>
--- a/combined_results.xlsx
+++ b/combined_results.xlsx
@@ -491,235 +491,235 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDT</t>
+          <t>BTC-USDT</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0004411738754373592</v>
+        <v>0.0002355707053659351</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01411756401433655</v>
+        <v>0.01154296456310222</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01455880211940544</v>
+        <v>0.01177856301531213</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>INJ-USDT</t>
+          <t>ADA-USDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.05204775381411873</v>
+        <v>0.01292478406153876</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03903581536059483</v>
+        <v>0.01339764201500563</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01301871440194559</v>
+        <v>0.02632582863304762</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>SOL-USDT</t>
+          <t>ETH-BTC</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001279263144434917</v>
+        <v>0.001883451990810638</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.002558526288851655</v>
+        <v>-0.001883451990810638</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.00127927950976802</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>TIA-USDT</t>
+          <t>LINK-USDT</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.09954717263574867</v>
+        <v>0.003358950932448884</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.09580479772463879</v>
+        <v>0.05777395603804681</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003746104051777412</v>
+        <v>0.06113496046382026</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>ADA-USDT</t>
+          <t>AVAX-USDT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003615596109617839</v>
+        <v>0.01247411620885526</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.05706353859963282</v>
+        <v>-0.02245340917596074</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.05344987502161686</v>
+        <v>-0.009980537951007755</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>BONK-USDT</t>
+          <t>RUNE-USDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1550753463911244</v>
+        <v>0.0269079412061455</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01348481272965852</v>
+        <v>-0.04372540445999391</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1688219603605964</v>
+        <v>-0.01682198970494792</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDT</t>
+          <t>BONK-USDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0002341355598200452</v>
+        <v>0.1621304632791797</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0002341355598200452</v>
+        <v>-0.0137983373003505</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.1485730080851455</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>FET-USDT</t>
+          <t>ETH-USDT</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.02742355683531852</v>
+        <v>0.0004437344692830818</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04113533525299301</v>
+        <v>-0.0004437344692830818</v>
       </c>
       <c r="E9" t="n">
-        <v>0.06857769853244493</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>ATOM-USDT</t>
+          <t>DOT-USDT</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.001774811869953413</v>
+        <v>0.01380357512596223</v>
       </c>
       <c r="D10" t="n">
-        <v>0.04437029674853583</v>
+        <v>0.09800538339429139</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04614592762189017</v>
+        <v>0.1118243942845278</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>DOT-USDT</t>
+          <t>SOL-USDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01099036968855919</v>
+        <v>0.003926958570587229</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01785935074391783</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02885289147191562</v>
+        <v>0.003927112786679382</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>MATIC-USDT</t>
+          <t>DOGE-USDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0115433452614555</v>
+        <v>0.02101281781887595</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.023086690522911</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.01154467790348522</v>
+        <v>0.02101723413199467</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDC</t>
+          <t>ATOM-USDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0004411797145663547</v>
+        <v>0.004472992073863511</v>
       </c>
       <c r="D13" t="n">
-        <v>0.003970617430996879</v>
+        <v>0.01431357463634417</v>
       </c>
       <c r="E13" t="n">
-        <v>0.004411816609603159</v>
+        <v>0.01878740706943678</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>AVAX-USDT</t>
+          <t>ETH-USDC</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.002460629921254108</v>
+        <v>0.002661910719512047</v>
       </c>
       <c r="D14" t="n">
-        <v>0.009842519685033914</v>
+        <v>0.04658343759151125</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01230345234871786</v>
+        <v>0.04924665921312389</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>XRP-USDT</t>
+          <t>MATIC-USDT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.001591444394943267</v>
+        <v>0.01161575095829817</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.001591444394943267</v>
+        <v>-0.01161575095829817</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -729,102 +729,102 @@
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>LINK-USDT</t>
+          <t>INJ-USDT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.004665204902464861</v>
+        <v>0.08347781416554229</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02865768725799674</v>
+        <v>-0.1091632954472564</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03332444681418809</v>
+        <v>-0.02570694087404457</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>RUNE-USDT</t>
+          <t>TIA-USDT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.005015883631502909</v>
+        <v>0.08548769969392764</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.003343922420992039</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.001672045078346266</v>
+        <v>0.08556084369103784</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDC</t>
+          <t>JTO-USDT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0002341613277849856</v>
+        <v>0.1519401589527811</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.01311303435614661</v>
+        <v>0.04517139860758508</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.01287890318577233</v>
+        <v>0.1974115049147247</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>DOGE-USDT</t>
+          <t>XRP-USDT</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0104504127913012</v>
+        <v>0.001601819667152367</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04180165116521932</v>
+        <v>0.05766550801711175</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05225752508360628</v>
+        <v>0.05926827705518237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>ETH-BTC</t>
+          <t>FET-USDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.001884090737811817</v>
+        <v>0.01381215469613108</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02072499811591692</v>
+        <v>0.1381215469613261</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02260951483750365</v>
+        <v>0.1519546898742906</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>JTO-USDT</t>
+          <t>BTC-USDC</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.1491679273827632</v>
+        <v>0.01012560459277558</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.02481089258699071</v>
+        <v>0.00777081282702856</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1245428127282233</v>
+        <v>0.01789822972377508</v>
       </c>
     </row>
     <row r="22">
@@ -839,10 +839,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.341380814060954e-05</v>
+        <v>2.355197178765182e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>-2.341380814060954e-05</v>
+        <v>-2.355197178765182e-05</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -852,34 +852,34 @@
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>SOLUSDT</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.0246123554024246</v>
+        <v>0.01307702366941953</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>-0.01307702366941953</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02461841457411402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>BONKUSDT</t>
+          <t>FETUSDT</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.03372681281618284</v>
+        <v>0.02762049440684684</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>-0.04143074161027026</v>
       </c>
       <c r="E24" t="n">
-        <v>0.03373819163292244</v>
+        <v>-0.01381406271584321</v>
       </c>
     </row>
     <row r="25">
@@ -890,78 +890,78 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02246820748640758</v>
+        <v>0.01905938140871321</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>-0.03659401230473261</v>
       </c>
       <c r="E25" t="n">
-        <v>0.02247325682437984</v>
+        <v>-0.01753797352528494</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>INJUSDT</t>
+          <t>BONKUSDT</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.02277681970520759</v>
+        <v>0.03441156228492158</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.02603065109165756</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.003254572674600239</v>
+        <v>0.03442340791737766</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>SOLUSDT</t>
+          <t>ADAUSDT</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.01279263144429463</v>
+        <v>0.01575795776868894</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.01279263144429463</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>0.01576044129237195</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>XRPUSDT</t>
+          <t>JTOUSDT</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.01591596371160098</v>
+        <v>0.02210921954455465</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0.01591849729385371</v>
+        <v>0.02211410880141988</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>BTCUSDC</t>
+          <t>ETHUSDC</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2.341400001442609e-05</v>
+        <v>0.001330595263976798</v>
       </c>
       <c r="D29" t="n">
-        <v>-2.341400001442609e-05</v>
+        <v>-0.001330595263976798</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -971,116 +971,116 @@
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDC</t>
+          <t>ETHUSDT</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.003088530521286989</v>
+        <v>0.0004435750373607078</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0172075271901135</v>
+        <v>-0.0004435750373607078</v>
       </c>
       <c r="E30" t="n">
-        <v>0.02029668458069857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>ADAUSDT</t>
+          <t>RUNEUSDT</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01571832756994483</v>
+        <v>0.01681520094165687</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01572079861656799</v>
+        <v>0.01681802892701537</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>JTOUSDT</t>
+          <t>MATICUSDT</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.01815431164902808</v>
+        <v>0.01161710037174593</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.01512859304085225</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.003026268006301024</v>
+        <v>0.01161845009875555</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>MATICUSDT</t>
+          <t>DOTUSDT</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.01154201292705321</v>
+        <v>0.01379310344828047</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>-0.04137931034482915</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0115433452614555</v>
+        <v>-0.02759001241550255</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>LINKUSDT</t>
+          <t>ATOMUSDT</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.006665777896288642</v>
+        <v>0.008942144326204469</v>
       </c>
       <c r="D34" t="n">
-        <v>0.006665777896276801</v>
+        <v>-0.02682643297862929</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01333244450370421</v>
+        <v>-0.01788588803434688</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>DOGEUSDT</t>
+          <t>ETHBTC</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01045150501671836</v>
+        <v>0.01883239171375341</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0.01045259747046736</v>
+        <v>0.0188359389715635</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDT</t>
+          <t>LINKUSDT</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.0004412283798190204</v>
+        <v>0.00671546571754379</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.0004412283798190204</v>
+        <v>-0.00671546571754379</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1090,14 +1090,14 @@
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>RUNEUSDT</t>
+          <t>DOGEUSDT</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01671681711802631</v>
+        <v>0.01049979000421042</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.01671681711802631</v>
+        <v>-0.01049979000421042</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1107,14 +1107,14 @@
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>DOTUSDT</t>
+          <t>XRPUSDT</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.01373815084490087</v>
+        <v>0.01601537475976762</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.01373815084490087</v>
+        <v>-0.01601537475976762</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1124,51 +1124,51 @@
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>ATOMUSDT</t>
+          <t>BTCUSDC</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.00887390185464057</v>
+        <v>4.709817543269348e-05</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>-0.007370864456390223</v>
       </c>
       <c r="E39" t="n">
-        <v>0.008874689385866575</v>
+        <v>-0.007323769730319446</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>FETUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.02743860611880615</v>
+        <v>0.02495632642874472</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.01371930305940307</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0137230684781102</v>
+        <v>0.0249625561657464</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>ETHBTC</t>
+          <t>INJUSDT</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.01883593897155043</v>
+        <v>0.009631127805066338</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.01883593897155043</v>
+        <v>-0.006420751870051829</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.003210685160205707</v>
       </c>
     </row>
   </sheetData>
@@ -1229,235 +1229,235 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDT</t>
+          <t>BTC-USDT</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0004411738754373592</v>
+        <v>0.0002355707053659351</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01411756401433655</v>
+        <v>0.01154296456310222</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01455880211940544</v>
+        <v>0.01177856301531213</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>INJ-USDT</t>
+          <t>ADA-USDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.05204775381411873</v>
+        <v>0.01292478406153876</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03903581536059483</v>
+        <v>0.01339764201500563</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01301871440194559</v>
+        <v>0.02632582863304762</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>SOL-USDT</t>
+          <t>ETH-BTC</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001279263144434917</v>
+        <v>0.001883451990810638</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.002558526288851655</v>
+        <v>-0.001883451990810638</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.00127927950976802</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>TIA-USDT</t>
+          <t>LINK-USDT</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.09954717263574867</v>
+        <v>0.003358950932448884</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.09580479772463879</v>
+        <v>0.05777395603804681</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003746104051777412</v>
+        <v>0.06113496046382026</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>ADA-USDT</t>
+          <t>AVAX-USDT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003615596109617839</v>
+        <v>0.01247411620885526</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.05706353859963282</v>
+        <v>-0.02245340917596074</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.05344987502161686</v>
+        <v>-0.009980537951007755</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>BONK-USDT</t>
+          <t>RUNE-USDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1550753463911244</v>
+        <v>0.0269079412061455</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01348481272965852</v>
+        <v>-0.04372540445999391</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1688219603605964</v>
+        <v>-0.01682198970494792</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDT</t>
+          <t>BONK-USDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0002341355598200452</v>
+        <v>0.1621304632791797</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0002341355598200452</v>
+        <v>-0.0137983373003505</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.1485730080851455</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>FET-USDT</t>
+          <t>ETH-USDT</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.02742355683531852</v>
+        <v>0.0004437344692830818</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04113533525299301</v>
+        <v>-0.0004437344692830818</v>
       </c>
       <c r="E9" t="n">
-        <v>0.06857769853244493</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>ATOM-USDT</t>
+          <t>DOT-USDT</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.001774811869953413</v>
+        <v>0.01380357512596223</v>
       </c>
       <c r="D10" t="n">
-        <v>0.04437029674853583</v>
+        <v>0.09800538339429139</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04614592762189017</v>
+        <v>0.1118243942845278</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>DOT-USDT</t>
+          <t>SOL-USDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01099036968855919</v>
+        <v>0.003926958570587229</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01785935074391783</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02885289147191562</v>
+        <v>0.003927112786679382</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>MATIC-USDT</t>
+          <t>DOGE-USDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0115433452614555</v>
+        <v>0.02101281781887595</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.023086690522911</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.01154467790348522</v>
+        <v>0.02101723413199467</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDC</t>
+          <t>ATOM-USDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0004411797145663547</v>
+        <v>0.004472992073863511</v>
       </c>
       <c r="D13" t="n">
-        <v>0.003970617430996879</v>
+        <v>0.01431357463634417</v>
       </c>
       <c r="E13" t="n">
-        <v>0.004411816609603159</v>
+        <v>0.01878740706943678</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>AVAX-USDT</t>
+          <t>ETH-USDC</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.002460629921254108</v>
+        <v>0.002661910719512047</v>
       </c>
       <c r="D14" t="n">
-        <v>0.009842519685033914</v>
+        <v>0.04658343759151125</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01230345234871786</v>
+        <v>0.04924665921312389</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>XRP-USDT</t>
+          <t>MATIC-USDT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.001591444394943267</v>
+        <v>0.01161575095829817</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.001591444394943267</v>
+        <v>-0.01161575095829817</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1467,102 +1467,102 @@
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>LINK-USDT</t>
+          <t>INJ-USDT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.004665204902464861</v>
+        <v>0.08347781416554229</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02865768725799674</v>
+        <v>-0.1091632954472564</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03332444681418809</v>
+        <v>-0.02570694087404457</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>RUNE-USDT</t>
+          <t>TIA-USDT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.005015883631502909</v>
+        <v>0.08548769969392764</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.003343922420992039</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.001672045078346266</v>
+        <v>0.08556084369103784</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDC</t>
+          <t>JTO-USDT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0002341613277849856</v>
+        <v>0.1519401589527811</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.01311303435614661</v>
+        <v>0.04517139860758508</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.01287890318577233</v>
+        <v>0.1974115049147247</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>DOGE-USDT</t>
+          <t>XRP-USDT</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0104504127913012</v>
+        <v>0.001601819667152367</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04180165116521932</v>
+        <v>0.05766550801711175</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05225752508360628</v>
+        <v>0.05926827705518237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>ETH-BTC</t>
+          <t>FET-USDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.001884090737811817</v>
+        <v>0.01381215469613108</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02072499811591692</v>
+        <v>0.1381215469613261</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02260951483750365</v>
+        <v>0.1519546898742906</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>JTO-USDT</t>
+          <t>BTC-USDC</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.1491679273827632</v>
+        <v>0.01012560459277558</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.02481089258699071</v>
+        <v>0.00777081282702856</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1245428127282233</v>
+        <v>0.01789822972377508</v>
       </c>
     </row>
   </sheetData>
@@ -1626,10 +1626,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.341380814060954e-05</v>
+        <v>2.355197178765182e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>-2.341380814060954e-05</v>
+        <v>-2.355197178765182e-05</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1639,34 +1639,34 @@
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>SOLUSDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0246123554024246</v>
+        <v>0.01307702366941953</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>-0.01307702366941953</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02461841457411402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>BONKUSDT</t>
+          <t>FETUSDT</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.03372681281618284</v>
+        <v>0.02762049440684684</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-0.04143074161027026</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03373819163292244</v>
+        <v>-0.01381406271584321</v>
       </c>
     </row>
     <row r="5">
@@ -1677,78 +1677,78 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.02246820748640758</v>
+        <v>0.01905938140871321</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>-0.03659401230473261</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02247325682437984</v>
+        <v>-0.01753797352528494</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>INJUSDT</t>
+          <t>BONKUSDT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.02277681970520759</v>
+        <v>0.03441156228492158</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.02603065109165756</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.003254572674600239</v>
+        <v>0.03442340791737766</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>SOLUSDT</t>
+          <t>ADAUSDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.01279263144429463</v>
+        <v>0.01575795776868894</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.01279263144429463</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.01576044129237195</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>XRPUSDT</t>
+          <t>JTOUSDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.01591596371160098</v>
+        <v>0.02210921954455465</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01591849729385371</v>
+        <v>0.02211410880141988</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>BTCUSDC</t>
+          <t>ETHUSDC</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.341400001442609e-05</v>
+        <v>0.001330595263976798</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.341400001442609e-05</v>
+        <v>-0.001330595263976798</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1758,116 +1758,116 @@
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDC</t>
+          <t>ETHUSDT</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.003088530521286989</v>
+        <v>0.0004435750373607078</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0172075271901135</v>
+        <v>-0.0004435750373607078</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02029668458069857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>ADAUSDT</t>
+          <t>RUNEUSDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01571832756994483</v>
+        <v>0.01681520094165687</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01572079861656799</v>
+        <v>0.01681802892701537</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>JTOUSDT</t>
+          <t>MATICUSDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.01815431164902808</v>
+        <v>0.01161710037174593</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.01512859304085225</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.003026268006301024</v>
+        <v>0.01161845009875555</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>MATICUSDT</t>
+          <t>DOTUSDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01154201292705321</v>
+        <v>0.01379310344828047</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>-0.04137931034482915</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0115433452614555</v>
+        <v>-0.02759001241550255</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>LINKUSDT</t>
+          <t>ATOMUSDT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.006665777896288642</v>
+        <v>0.008942144326204469</v>
       </c>
       <c r="D14" t="n">
-        <v>0.006665777896276801</v>
+        <v>-0.02682643297862929</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01333244450370421</v>
+        <v>-0.01788588803434688</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>DOGEUSDT</t>
+          <t>ETHBTC</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01045150501671836</v>
+        <v>0.01883239171375341</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01045259747046736</v>
+        <v>0.0188359389715635</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDT</t>
+          <t>LINKUSDT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0004412283798190204</v>
+        <v>0.00671546571754379</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0004412283798190204</v>
+        <v>-0.00671546571754379</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1877,14 +1877,14 @@
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>RUNEUSDT</t>
+          <t>DOGEUSDT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01671681711802631</v>
+        <v>0.01049979000421042</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.01671681711802631</v>
+        <v>-0.01049979000421042</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1894,14 +1894,14 @@
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>DOTUSDT</t>
+          <t>XRPUSDT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.01373815084490087</v>
+        <v>0.01601537475976762</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.01373815084490087</v>
+        <v>-0.01601537475976762</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1911,51 +1911,51 @@
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>ATOMUSDT</t>
+          <t>BTCUSDC</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.00887390185464057</v>
+        <v>4.709817543269348e-05</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>-0.007370864456390223</v>
       </c>
       <c r="E19" t="n">
-        <v>0.008874689385866575</v>
+        <v>-0.007323769730319446</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>FETUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.02743860611880615</v>
+        <v>0.02495632642874472</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.01371930305940307</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0137230684781102</v>
+        <v>0.0249625561657464</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>ETHBTC</t>
+          <t>INJUSDT</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.01883593897155043</v>
+        <v>0.009631127805066338</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.01883593897155043</v>
+        <v>-0.006420751870051829</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.003210685160205707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store results in a sqlite3 database
</commit_message>
<xml_diff>
--- a/combined_results.xlsx
+++ b/combined_results.xlsx
@@ -495,336 +495,336 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0002355707053659351</v>
+        <v>0.0002329612166132676</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01154296456310222</v>
+        <v>-0.0002329612166132676</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01177856301531213</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>ADA-USDT</t>
+          <t>ETH-USDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01292478406153876</v>
+        <v>0.0004516079500956745</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01339764201500563</v>
+        <v>-0.0004516079500956745</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02632582863304762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>ETH-BTC</t>
+          <t>INJ-USDT</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001883451990810638</v>
+        <v>0.09479824987846737</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.001883451990810638</v>
+        <v>-0.06319883325231734</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.03162940074450287</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>LINK-USDT</t>
+          <t>AVAX-USDT</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003358950932448884</v>
+        <v>0.002406275566672288</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05777395603804681</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06113496046382026</v>
+        <v>0.002406333469686622</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>AVAX-USDT</t>
+          <t>BTC-USDC</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.01247411620885526</v>
+        <v>0.0002330714387402507</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.02245340917596074</v>
+        <v>0.03099850135063881</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.009980537951007755</v>
+        <v>0.03123164558142476</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>RUNE-USDT</t>
+          <t>SOL-USDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0269079412061455</v>
+        <v>0.01711066652627834</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.04372540445999391</v>
+        <v>-0.01184584605664992</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.01682198970494792</v>
+        <v>0.005265721469669298</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>BONK-USDT</t>
+          <t>FET-USDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1621304632791797</v>
+        <v>0.02802690582959333</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0137983373003505</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1485730080851455</v>
+        <v>0.02803476310624866</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDT</t>
+          <t>DOGE-USDT</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0004437344692830818</v>
+        <v>0.01106194690265058</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0004437344692830818</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.01106317070471968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>DOT-USDT</t>
+          <t>ETH-USDC</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.01380357512596223</v>
+        <v>0.0004518957024817334</v>
       </c>
       <c r="D10" t="n">
-        <v>0.09800538339429139</v>
+        <v>0.01310497537168257</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1118243942845278</v>
+        <v>0.01355693233735893</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>SOL-USDT</t>
+          <t>ADA-USDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.003926958570587229</v>
+        <v>0.01119013911377667</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.0003390951246507725</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003927112786679382</v>
+        <v>0.0115305245201618</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>DOGE-USDT</t>
+          <t>MATIC-USDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.02101281781887595</v>
+        <v>0.01286504567091071</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.02573009134182143</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02101723413199467</v>
+        <v>0.03860010293360357</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ATOM-USDT</t>
+          <t>RUNE-USDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.004472992073863511</v>
+        <v>0.001886685659297907</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01431357463634417</v>
+        <v>0.01698017093371467</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01878740706943678</v>
+        <v>0.01886721255800622</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDC</t>
+          <t>BONK-USDT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.002661910719512047</v>
+        <v>0.06707282991447772</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04658343759151125</v>
+        <v>0.005589402492885768</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04924665921312389</v>
+        <v>0.07271100173388557</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>MATIC-USDT</t>
+          <t>LINK-USDT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01161575095829817</v>
+        <v>0.0006948352892930534</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.01161575095829817</v>
+        <v>-0.001389670578586107</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>-0.0006948401172873924</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>INJ-USDT</t>
+          <t>ATOM-USDT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.08347781416554229</v>
+        <v>0.0009400616680599317</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1091632954472564</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.02570694087404457</v>
+        <v>0.0009400705053024047</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>TIA-USDT</t>
+          <t>ETH-BTC</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.08548769969392764</v>
+        <v>0.001938548027529321</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08556084369103784</v>
+        <v>0.001938585607942385</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>JTO-USDT</t>
+          <t>TIA-USDT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1519401589527811</v>
+        <v>0.09351052785899837</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04517139860758508</v>
+        <v>-0.04517033972849575</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1974115049147247</v>
+        <v>0.04838543360487339</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>XRP-USDT</t>
+          <t>JTO-USDT</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.001601819667152367</v>
+        <v>0.1384962565276573</v>
       </c>
       <c r="D19" t="n">
-        <v>0.05766550801711175</v>
+        <v>-0.02484785778878504</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05926827705518237</v>
+        <v>0.113806015810473</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>FET-USDT</t>
+          <t>XRP-USDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.01381215469613108</v>
+        <v>0.001640070194996882</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1381215469613261</v>
+        <v>-0.008200350975020828</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1519546898742906</v>
+        <v>-0.00656038837499836</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDC</t>
+          <t>DOT-USDT</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.01012560459277558</v>
+        <v>0.04787673915881171</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00777081282702856</v>
+        <v>0.02321296444065043</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01789822972377508</v>
+        <v>0.07112375533428349</v>
       </c>
     </row>
     <row r="22">
@@ -839,336 +839,336 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.355197178765182e-05</v>
+        <v>2.329487350193526e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>-2.355197178765182e-05</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2.329487892844784e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>SOLUSDT</t>
+          <t>ETHUSDT</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.01307702366941953</v>
+        <v>0.0004516099896228279</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.01307702366941953</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.0004516120291478658</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>FETUSDT</t>
+          <t>SOLUSDT</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.02762049440684684</v>
+        <v>0.01316309069370161</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.04143074161027026</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.01381406271584321</v>
+        <v>0.01316482359137061</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>TIAUSDT</t>
+          <t>BTCUSDC</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.01905938140871321</v>
+        <v>2.330782292589456e-05</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.03659401230473261</v>
+        <v>-0.0001864625833732392</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.01753797352528494</v>
+        <v>-0.0001631547984751761</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>BONKUSDT</t>
+          <t>INJUSDT</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.03441156228492158</v>
+        <v>0.0121616033857966</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>-0.009729282708626915</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03442340791737766</v>
+        <v>0.002432616522343035</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>ADAUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.01575795776868894</v>
+        <v>0.024044241404196</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>-0.024044241404196</v>
       </c>
       <c r="E27" t="n">
-        <v>0.01576044129237195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>JTOUSDT</t>
+          <t>ADAUSDT</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.02210921954455465</v>
+        <v>0.0169520257670773</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>-0.0169520257670773</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02211410880141988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDC</t>
+          <t>TIAUSDT</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.001330595263976798</v>
+        <v>0.03962624525476333</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.001330595263976798</v>
+        <v>-0.00317009962038726</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.03647059756281218</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDT</t>
+          <t>BONKUSDT</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.0004435750373607078</v>
+        <v>0.05586592178771842</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0004435750373607078</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>0.05589714924539742</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>RUNEUSDT</t>
+          <t>XRPUSDT</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01681520094165687</v>
+        <v>0.01640419947506381</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>-0.01640419947506381</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01681802892701537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>MATICUSDT</t>
+          <t>JTOUSDT</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.01161710037174593</v>
+        <v>0.02038403522361967</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>0.004076807044713072</v>
       </c>
       <c r="E32" t="n">
-        <v>0.01161845009875555</v>
+        <v>0.02446582939161368</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>DOTUSDT</t>
+          <t>RUNEUSDT</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.01379310344828047</v>
+        <v>0.01886436521411684</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.04137931034482915</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.02759001241550255</v>
+        <v>0.01886792452830819</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>ATOMUSDT</t>
+          <t>DOGEUSDT</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.008942144326204469</v>
+        <v>0.01106194690265058</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.02682643297862929</v>
+        <v>-0.02212389380530116</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.01788588803434688</v>
+        <v>-0.01106317070471968</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>ETHBTC</t>
+          <t>LINKUSDT</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01883239171375341</v>
+        <v>0.00694637399278426</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>-0.0208391219783281</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0188359389715635</v>
+        <v>-0.01389371309481689</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>LINKUSDT</t>
+          <t>ETHUSDC</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.00671546571754379</v>
+        <v>0.0004518609894950579</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.00671546571754379</v>
+        <v>0.009489080779190733</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.009940986688126605</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>DOGEUSDT</t>
+          <t>FETUSDT</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01049979000421042</v>
+        <v>0.02801120448178964</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.01049979000421042</v>
+        <v>-0.01400560224089482</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>0.0140095264780035</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>XRPUSDT</t>
+          <t>ETHBTC</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.01601537475976762</v>
+        <v>0.0193836014731462</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.01601537475976762</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>0.01938735944163653</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>BTCUSDC</t>
+          <t>ATOMUSDT</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4.709817543269348e-05</v>
+        <v>0.009395847035621744</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.007370864456390223</v>
+        <v>-0.0187916940712268</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.007323769730319446</v>
+        <v>-0.009396729937976375</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>MATICUSDT</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.02495632642874472</v>
+        <v>0.01286008230452533</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>-0.01286008230452533</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0249625561657464</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>INJUSDT</t>
+          <t>DOTUSDT</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.009631127805066338</v>
+        <v>0.01450747134773605</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.006420751870051829</v>
+        <v>-0.01450747134773605</v>
       </c>
       <c r="E41" t="n">
-        <v>0.003210685160205707</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1233,336 +1233,336 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0002355707053659351</v>
+        <v>0.0002329612166132676</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01154296456310222</v>
+        <v>-0.0002329612166132676</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01177856301531213</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>ADA-USDT</t>
+          <t>ETH-USDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01292478406153876</v>
+        <v>0.0004516079500956745</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01339764201500563</v>
+        <v>-0.0004516079500956745</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02632582863304762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>ETH-BTC</t>
+          <t>INJ-USDT</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001883451990810638</v>
+        <v>0.09479824987846737</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.001883451990810638</v>
+        <v>-0.06319883325231734</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.03162940074450287</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>LINK-USDT</t>
+          <t>AVAX-USDT</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003358950932448884</v>
+        <v>0.002406275566672288</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05777395603804681</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06113496046382026</v>
+        <v>0.002406333469686622</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>AVAX-USDT</t>
+          <t>BTC-USDC</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.01247411620885526</v>
+        <v>0.0002330714387402507</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.02245340917596074</v>
+        <v>0.03099850135063881</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.009980537951007755</v>
+        <v>0.03123164558142476</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>RUNE-USDT</t>
+          <t>SOL-USDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0269079412061455</v>
+        <v>0.01711066652627834</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.04372540445999391</v>
+        <v>-0.01184584605664992</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.01682198970494792</v>
+        <v>0.005265721469669298</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>BONK-USDT</t>
+          <t>FET-USDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1621304632791797</v>
+        <v>0.02802690582959333</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0137983373003505</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1485730080851455</v>
+        <v>0.02803476310624866</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDT</t>
+          <t>DOGE-USDT</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0004437344692830818</v>
+        <v>0.01106194690265058</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0004437344692830818</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.01106317070471968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>DOT-USDT</t>
+          <t>ETH-USDC</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.01380357512596223</v>
+        <v>0.0004518957024817334</v>
       </c>
       <c r="D10" t="n">
-        <v>0.09800538339429139</v>
+        <v>0.01310497537168257</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1118243942845278</v>
+        <v>0.01355693233735893</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>SOL-USDT</t>
+          <t>ADA-USDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.003926958570587229</v>
+        <v>0.01119013911377667</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.0003390951246507725</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003927112786679382</v>
+        <v>0.0115305245201618</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>DOGE-USDT</t>
+          <t>MATIC-USDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.02101281781887595</v>
+        <v>0.01286504567091071</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.02573009134182143</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02101723413199467</v>
+        <v>0.03860010293360357</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>ATOM-USDT</t>
+          <t>RUNE-USDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.004472992073863511</v>
+        <v>0.001886685659297907</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01431357463634417</v>
+        <v>0.01698017093371467</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01878740706943678</v>
+        <v>0.01886721255800622</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>ETH-USDC</t>
+          <t>BONK-USDT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.002661910719512047</v>
+        <v>0.06707282991447772</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04658343759151125</v>
+        <v>0.005589402492885768</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04924665921312389</v>
+        <v>0.07271100173388557</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>MATIC-USDT</t>
+          <t>LINK-USDT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01161575095829817</v>
+        <v>0.0006948352892930534</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.01161575095829817</v>
+        <v>-0.001389670578586107</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>-0.0006948401172873924</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>INJ-USDT</t>
+          <t>ATOM-USDT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.08347781416554229</v>
+        <v>0.0009400616680599317</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1091632954472564</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.02570694087404457</v>
+        <v>0.0009400705053024047</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>TIA-USDT</t>
+          <t>ETH-BTC</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.08548769969392764</v>
+        <v>0.001938548027529321</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08556084369103784</v>
+        <v>0.001938585607942385</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>JTO-USDT</t>
+          <t>TIA-USDT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1519401589527811</v>
+        <v>0.09351052785899837</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04517139860758508</v>
+        <v>-0.04517033972849575</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1974115049147247</v>
+        <v>0.04838543360487339</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>XRP-USDT</t>
+          <t>JTO-USDT</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.001601819667152367</v>
+        <v>0.1384962565276573</v>
       </c>
       <c r="D19" t="n">
-        <v>0.05766550801711175</v>
+        <v>-0.02484785778878504</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05926827705518237</v>
+        <v>0.113806015810473</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>FET-USDT</t>
+          <t>XRP-USDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.01381215469613108</v>
+        <v>0.001640070194996882</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1381215469613261</v>
+        <v>-0.008200350975020828</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1519546898742906</v>
+        <v>-0.00656038837499836</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>BTC-USDC</t>
+          <t>DOT-USDT</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.01012560459277558</v>
+        <v>0.04787673915881171</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00777081282702856</v>
+        <v>0.02321296444065043</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01789822972377508</v>
+        <v>0.07112375533428349</v>
       </c>
     </row>
   </sheetData>
@@ -1626,336 +1626,336 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.355197178765182e-05</v>
+        <v>2.329487350193526e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>-2.355197178765182e-05</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.329487892844784e-05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>SOLUSDT</t>
+          <t>ETHUSDT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01307702366941953</v>
+        <v>0.0004516099896228279</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.01307702366941953</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.0004516120291478658</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>FETUSDT</t>
+          <t>SOLUSDT</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.02762049440684684</v>
+        <v>0.01316309069370161</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.04143074161027026</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.01381406271584321</v>
+        <v>0.01316482359137061</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>TIAUSDT</t>
+          <t>BTCUSDC</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01905938140871321</v>
+        <v>2.330782292589456e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.03659401230473261</v>
+        <v>-0.0001864625833732392</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.01753797352528494</v>
+        <v>-0.0001631547984751761</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>BONKUSDT</t>
+          <t>INJUSDT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.03441156228492158</v>
+        <v>0.0121616033857966</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>-0.009729282708626915</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03442340791737766</v>
+        <v>0.002432616522343035</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>ADAUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.01575795776868894</v>
+        <v>0.024044241404196</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>-0.024044241404196</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01576044129237195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>JTOUSDT</t>
+          <t>ADAUSDT</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.02210921954455465</v>
+        <v>0.0169520257670773</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>-0.0169520257670773</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02211410880141988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDC</t>
+          <t>TIAUSDT</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.001330595263976798</v>
+        <v>0.03962624525476333</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.001330595263976798</v>
+        <v>-0.00317009962038726</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.03647059756281218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>ETHUSDT</t>
+          <t>BONKUSDT</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0004435750373607078</v>
+        <v>0.05586592178771842</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0004435750373607078</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.05589714924539742</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>RUNEUSDT</t>
+          <t>XRPUSDT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01681520094165687</v>
+        <v>0.01640419947506381</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>-0.01640419947506381</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01681802892701537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>MATICUSDT</t>
+          <t>JTOUSDT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.01161710037174593</v>
+        <v>0.02038403522361967</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.004076807044713072</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01161845009875555</v>
+        <v>0.02446582939161368</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>DOTUSDT</t>
+          <t>RUNEUSDT</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01379310344828047</v>
+        <v>0.01886436521411684</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04137931034482915</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.02759001241550255</v>
+        <v>0.01886792452830819</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>ATOMUSDT</t>
+          <t>DOGEUSDT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.008942144326204469</v>
+        <v>0.01106194690265058</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.02682643297862929</v>
+        <v>-0.02212389380530116</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01788588803434688</v>
+        <v>-0.01106317070471968</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>ETHBTC</t>
+          <t>LINKUSDT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.01883239171375341</v>
+        <v>0.00694637399278426</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>-0.0208391219783281</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0188359389715635</v>
+        <v>-0.01389371309481689</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>LINKUSDT</t>
+          <t>ETHUSDC</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.00671546571754379</v>
+        <v>0.0004518609894950579</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.00671546571754379</v>
+        <v>0.009489080779190733</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.009940986688126605</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>DOGEUSDT</t>
+          <t>FETUSDT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01049979000421042</v>
+        <v>0.02801120448178964</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.01049979000421042</v>
+        <v>-0.01400560224089482</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.0140095264780035</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>XRPUSDT</t>
+          <t>ETHBTC</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.01601537475976762</v>
+        <v>0.0193836014731462</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.01601537475976762</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.01938735944163653</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>BTCUSDC</t>
+          <t>ATOMUSDT</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.709817543269348e-05</v>
+        <v>0.009395847035621744</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.007370864456390223</v>
+        <v>-0.0187916940712268</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.007323769730319446</v>
+        <v>-0.009396729937976375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>MATICUSDT</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.02495632642874472</v>
+        <v>0.01286008230452533</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>-0.01286008230452533</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0249625561657464</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>INJUSDT</t>
+          <t>DOTUSDT</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.009631127805066338</v>
+        <v>0.01450747134773605</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.006420751870051829</v>
+        <v>-0.01450747134773605</v>
       </c>
       <c r="E21" t="n">
-        <v>0.003210685160205707</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>